<commit_message>
Estuve organizando un poco la información como les dije para tener las listas en un solo lugar
Tambien ya estoy implementando los diccionarios, en particular implementé los de nombres y ciudades. Siendo nuestro diccionario de ciudades tan completo y el de nombres tan incompleto, muchos nombres se etiquetaban como ciudades. A Gerardo no le gustó y por lo mientras el diccionario de Ciudades está apagado.

El trabajo fuerte ahora se está haciendo en el archivo de tags.py, encontré unos patrones muy recurrentes para nombres, y al menos eso parece que ya está funcionando bastante bien, pueden ver un resultado en resultado.flg
</commit_message>
<xml_diff>
--- a/jerarquía de etiquetas.xlsx
+++ b/jerarquía de etiquetas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Nombre de la etiqueta</t>
   </si>
@@ -39,15 +39,9 @@
     <t>servicios públicos</t>
   </si>
   <si>
-    <t>localidades</t>
-  </si>
-  <si>
     <t>NE00P00</t>
   </si>
   <si>
-    <t>NE00L00</t>
-  </si>
-  <si>
     <t>NE00O00</t>
   </si>
   <si>
@@ -61,6 +55,21 @@
   </si>
   <si>
     <t>Aquí trataré de hacer una lista, pero no será para nada suficiente</t>
+  </si>
+  <si>
+    <t>* Por ahora esta categoría se maneja de manera independiente</t>
+  </si>
+  <si>
+    <t>NE00U00</t>
+  </si>
+  <si>
+    <t>NE00C00</t>
+  </si>
+  <si>
+    <t>ubicaciones</t>
+  </si>
+  <si>
+    <t>*No tenemos diccionarios de ubicaciones</t>
   </si>
 </sst>
 </file>
@@ -521,7 +530,7 @@
   <dimension ref="A3:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +543,7 @@
   <sheetData>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -545,7 +554,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -556,7 +565,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -568,19 +577,22 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C9" si="0">C5+1</f>
         <v>3</v>
       </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -592,7 +604,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -602,12 +614,12 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -615,6 +627,9 @@
       <c r="C9">
         <f t="shared" si="0"/>
         <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>